<commit_message>
need correct date in laps and drivers saved
</commit_message>
<xml_diff>
--- a/telemetry_data/4/4_telemetry_laps_9955.xlsx
+++ b/telemetry_data/4/4_telemetry_laps_9955.xlsx
@@ -16,7 +16,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +60,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P71"/>
+  <dimension ref="A1:R71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,10 +521,20 @@
           <t>st_speed</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>date_only</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>time_only</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1264</v>
+      <c r="A2" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B2" t="n">
         <v>9955</v>
@@ -564,10 +581,18 @@
       <c r="P2" t="n">
         <v>293</v>
       </c>
+      <c r="Q2" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>1264</v>
+      <c r="A3" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B3" t="n">
         <v>9955</v>
@@ -622,10 +647,18 @@
       <c r="P3" t="n">
         <v>165</v>
       </c>
+      <c r="Q3" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>1264</v>
+      <c r="A4" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B4" t="n">
         <v>9955</v>
@@ -680,10 +713,18 @@
       <c r="P4" t="n">
         <v>172</v>
       </c>
+      <c r="Q4" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>1264</v>
+      <c r="A5" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B5" t="n">
         <v>9955</v>
@@ -738,10 +779,18 @@
       <c r="P5" t="n">
         <v>295</v>
       </c>
+      <c r="Q5" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>1264</v>
+      <c r="A6" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B6" t="n">
         <v>9955</v>
@@ -796,10 +845,18 @@
       <c r="P6" t="n">
         <v>281</v>
       </c>
+      <c r="Q6" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>1264</v>
+      <c r="A7" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B7" t="n">
         <v>9955</v>
@@ -854,10 +911,18 @@
       <c r="P7" t="n">
         <v>288</v>
       </c>
+      <c r="Q7" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>1264</v>
+      <c r="A8" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B8" t="n">
         <v>9955</v>
@@ -912,10 +977,18 @@
       <c r="P8" t="n">
         <v>286</v>
       </c>
+      <c r="Q8" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>1264</v>
+      <c r="A9" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B9" t="n">
         <v>9955</v>
@@ -970,10 +1043,18 @@
       <c r="P9" t="n">
         <v>288</v>
       </c>
+      <c r="Q9" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>1264</v>
+      <c r="A10" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B10" t="n">
         <v>9955</v>
@@ -1028,10 +1109,18 @@
       <c r="P10" t="n">
         <v>293</v>
       </c>
+      <c r="Q10" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>1264</v>
+      <c r="A11" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B11" t="n">
         <v>9955</v>
@@ -1084,10 +1173,18 @@
       <c r="P11" t="n">
         <v>293</v>
       </c>
+      <c r="Q11" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>1264</v>
+      <c r="A12" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B12" t="n">
         <v>9955</v>
@@ -1140,10 +1237,18 @@
       <c r="P12" t="n">
         <v>290</v>
       </c>
+      <c r="Q12" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>1264</v>
+      <c r="A13" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B13" t="n">
         <v>9955</v>
@@ -1196,10 +1301,18 @@
       <c r="P13" t="n">
         <v>294</v>
       </c>
+      <c r="Q13" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>1264</v>
+      <c r="A14" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B14" t="n">
         <v>9955</v>
@@ -1254,10 +1367,18 @@
       <c r="P14" t="n">
         <v>293</v>
       </c>
+      <c r="Q14" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>1264</v>
+      <c r="A15" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B15" t="n">
         <v>9955</v>
@@ -1312,10 +1433,18 @@
       <c r="P15" t="n">
         <v>288</v>
       </c>
+      <c r="Q15" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>1264</v>
+      <c r="A16" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B16" t="n">
         <v>9955</v>
@@ -1368,10 +1497,18 @@
       <c r="P16" t="n">
         <v>297</v>
       </c>
+      <c r="Q16" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>1264</v>
+      <c r="A17" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B17" t="n">
         <v>9955</v>
@@ -1426,10 +1563,18 @@
       <c r="P17" t="n">
         <v>288</v>
       </c>
+      <c r="Q17" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>1264</v>
+      <c r="A18" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B18" t="n">
         <v>9955</v>
@@ -1484,10 +1629,18 @@
       <c r="P18" t="n">
         <v>285</v>
       </c>
+      <c r="Q18" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>1264</v>
+      <c r="A19" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B19" t="n">
         <v>9955</v>
@@ -1542,10 +1695,18 @@
       <c r="P19" t="n">
         <v>290</v>
       </c>
+      <c r="Q19" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>1264</v>
+      <c r="A20" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B20" t="n">
         <v>9955</v>
@@ -1600,10 +1761,18 @@
       <c r="P20" t="n">
         <v>289</v>
       </c>
+      <c r="Q20" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>1264</v>
+      <c r="A21" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B21" t="n">
         <v>9955</v>
@@ -1658,10 +1827,18 @@
       <c r="P21" t="n">
         <v>297</v>
       </c>
+      <c r="Q21" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>1264</v>
+      <c r="A22" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B22" t="n">
         <v>9955</v>
@@ -1716,10 +1893,18 @@
       <c r="P22" t="n">
         <v>290</v>
       </c>
+      <c r="Q22" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>1264</v>
+      <c r="A23" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B23" t="n">
         <v>9955</v>
@@ -1774,10 +1959,18 @@
       <c r="P23" t="n">
         <v>288</v>
       </c>
+      <c r="Q23" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>1264</v>
+      <c r="A24" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B24" t="n">
         <v>9955</v>
@@ -1832,10 +2025,18 @@
       <c r="P24" t="n">
         <v>288</v>
       </c>
+      <c r="Q24" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>1264</v>
+      <c r="A25" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B25" t="n">
         <v>9955</v>
@@ -1888,10 +2089,18 @@
       <c r="P25" t="n">
         <v>289</v>
       </c>
+      <c r="Q25" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>1264</v>
+      <c r="A26" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B26" t="n">
         <v>9955</v>
@@ -1946,10 +2155,18 @@
       <c r="P26" t="n">
         <v>294</v>
       </c>
+      <c r="Q26" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>1264</v>
+      <c r="A27" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B27" t="n">
         <v>9955</v>
@@ -2004,10 +2221,18 @@
       <c r="P27" t="n">
         <v>294</v>
       </c>
+      <c r="Q27" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>1264</v>
+      <c r="A28" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B28" t="n">
         <v>9955</v>
@@ -2062,10 +2287,18 @@
       <c r="P28" t="n">
         <v>294</v>
       </c>
+      <c r="Q28" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>1264</v>
+      <c r="A29" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B29" t="n">
         <v>9955</v>
@@ -2120,10 +2353,18 @@
       <c r="P29" t="n">
         <v>294</v>
       </c>
+      <c r="Q29" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>1264</v>
+      <c r="A30" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B30" t="n">
         <v>9955</v>
@@ -2176,10 +2417,18 @@
       <c r="P30" t="n">
         <v>294</v>
       </c>
+      <c r="Q30" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
-        <v>1264</v>
+      <c r="A31" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B31" t="n">
         <v>9955</v>
@@ -2232,10 +2481,18 @@
       <c r="P31" t="n">
         <v>294</v>
       </c>
+      <c r="Q31" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
-        <v>1264</v>
+      <c r="A32" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B32" t="n">
         <v>9955</v>
@@ -2290,10 +2547,18 @@
       <c r="P32" t="n">
         <v>294</v>
       </c>
+      <c r="Q32" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
-        <v>1264</v>
+      <c r="A33" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B33" t="n">
         <v>9955</v>
@@ -2346,10 +2611,18 @@
       <c r="P33" t="n">
         <v>291</v>
       </c>
+      <c r="Q33" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
-        <v>1264</v>
+      <c r="A34" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B34" t="n">
         <v>9955</v>
@@ -2402,10 +2675,18 @@
       <c r="P34" t="n">
         <v>294</v>
       </c>
+      <c r="Q34" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
-        <v>1264</v>
+      <c r="A35" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B35" t="n">
         <v>9955</v>
@@ -2460,10 +2741,18 @@
       <c r="P35" t="n">
         <v>293</v>
       </c>
+      <c r="Q35" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
-        <v>1264</v>
+      <c r="A36" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B36" t="n">
         <v>9955</v>
@@ -2516,10 +2805,18 @@
       <c r="P36" t="n">
         <v>296</v>
       </c>
+      <c r="Q36" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
-        <v>1264</v>
+      <c r="A37" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B37" t="n">
         <v>9955</v>
@@ -2574,10 +2871,18 @@
       <c r="P37" t="n">
         <v>296</v>
       </c>
+      <c r="Q37" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
-        <v>1264</v>
+      <c r="A38" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B38" t="n">
         <v>9955</v>
@@ -2632,10 +2937,18 @@
       <c r="P38" t="n">
         <v>298</v>
       </c>
+      <c r="Q38" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
-        <v>1264</v>
+      <c r="A39" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B39" t="n">
         <v>9955</v>
@@ -2690,10 +3003,18 @@
       <c r="P39" t="n">
         <v>295</v>
       </c>
+      <c r="Q39" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
-        <v>1264</v>
+      <c r="A40" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B40" t="n">
         <v>9955</v>
@@ -2748,10 +3069,18 @@
       <c r="P40" t="n">
         <v>298</v>
       </c>
+      <c r="Q40" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
-        <v>1264</v>
+      <c r="A41" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B41" t="n">
         <v>9955</v>
@@ -2806,10 +3135,18 @@
       <c r="P41" t="n">
         <v>301</v>
       </c>
+      <c r="Q41" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
-        <v>1264</v>
+      <c r="A42" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B42" t="n">
         <v>9955</v>
@@ -2864,10 +3201,18 @@
       <c r="P42" t="n">
         <v>296</v>
       </c>
+      <c r="Q42" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>1264</v>
+      <c r="A43" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B43" t="n">
         <v>9955</v>
@@ -2922,10 +3267,18 @@
       <c r="P43" t="n">
         <v>295</v>
       </c>
+      <c r="Q43" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
-        <v>1264</v>
+      <c r="A44" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B44" t="n">
         <v>9955</v>
@@ -2980,10 +3333,18 @@
       <c r="P44" t="n">
         <v>297</v>
       </c>
+      <c r="Q44" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>1264</v>
+      <c r="A45" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B45" t="n">
         <v>9955</v>
@@ -3038,10 +3399,18 @@
       <c r="P45" t="n">
         <v>296</v>
       </c>
+      <c r="Q45" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
-        <v>1264</v>
+      <c r="A46" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B46" t="n">
         <v>9955</v>
@@ -3096,10 +3465,18 @@
       <c r="P46" t="n">
         <v>290</v>
       </c>
+      <c r="Q46" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
-        <v>1264</v>
+      <c r="A47" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B47" t="n">
         <v>9955</v>
@@ -3154,10 +3531,18 @@
       <c r="P47" t="n">
         <v>296</v>
       </c>
+      <c r="Q47" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
-        <v>1264</v>
+      <c r="A48" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B48" t="n">
         <v>9955</v>
@@ -3210,10 +3595,18 @@
       <c r="P48" t="n">
         <v>298</v>
       </c>
+      <c r="Q48" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
-        <v>1264</v>
+      <c r="A49" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B49" t="n">
         <v>9955</v>
@@ -3268,10 +3661,18 @@
       <c r="P49" t="n">
         <v>298</v>
       </c>
+      <c r="Q49" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
-        <v>1264</v>
+      <c r="A50" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B50" t="n">
         <v>9955</v>
@@ -3324,10 +3725,18 @@
       <c r="P50" t="n">
         <v>297</v>
       </c>
+      <c r="Q50" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
-        <v>1264</v>
+      <c r="A51" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B51" t="n">
         <v>9955</v>
@@ -3382,10 +3791,18 @@
       <c r="P51" t="n">
         <v>298</v>
       </c>
+      <c r="Q51" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" t="n">
-        <v>1264</v>
+      <c r="A52" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B52" t="n">
         <v>9955</v>
@@ -3440,10 +3857,18 @@
       <c r="P52" t="n">
         <v>299</v>
       </c>
+      <c r="Q52" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="53">
-      <c r="A53" t="n">
-        <v>1264</v>
+      <c r="A53" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B53" t="n">
         <v>9955</v>
@@ -3498,10 +3923,18 @@
       <c r="P53" t="n">
         <v>299</v>
       </c>
+      <c r="Q53" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="54">
-      <c r="A54" t="n">
-        <v>1264</v>
+      <c r="A54" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B54" t="n">
         <v>9955</v>
@@ -3556,10 +3989,18 @@
       <c r="P54" t="n">
         <v>295</v>
       </c>
+      <c r="Q54" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" t="n">
-        <v>1264</v>
+      <c r="A55" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B55" t="n">
         <v>9955</v>
@@ -3614,10 +4055,18 @@
       <c r="P55" t="n">
         <v>299</v>
       </c>
+      <c r="Q55" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="56">
-      <c r="A56" t="n">
-        <v>1264</v>
+      <c r="A56" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B56" t="n">
         <v>9955</v>
@@ -3670,10 +4119,18 @@
       <c r="P56" t="n">
         <v>296</v>
       </c>
+      <c r="Q56" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="57">
-      <c r="A57" t="n">
-        <v>1264</v>
+      <c r="A57" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B57" t="n">
         <v>9955</v>
@@ -3728,10 +4185,18 @@
       <c r="P57" t="n">
         <v>298</v>
       </c>
+      <c r="Q57" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="58">
-      <c r="A58" t="n">
-        <v>1264</v>
+      <c r="A58" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B58" t="n">
         <v>9955</v>
@@ -3784,10 +4249,18 @@
       <c r="P58" t="n">
         <v>298</v>
       </c>
+      <c r="Q58" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" t="n">
-        <v>1264</v>
+      <c r="A59" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B59" t="n">
         <v>9955</v>
@@ -3842,10 +4315,18 @@
       <c r="P59" t="n">
         <v>300</v>
       </c>
+      <c r="Q59" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" t="n">
-        <v>1264</v>
+      <c r="A60" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B60" t="n">
         <v>9955</v>
@@ -3900,10 +4381,18 @@
       <c r="P60" t="n">
         <v>299</v>
       </c>
+      <c r="Q60" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="61">
-      <c r="A61" t="n">
-        <v>1264</v>
+      <c r="A61" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B61" t="n">
         <v>9955</v>
@@ -3958,10 +4447,18 @@
       <c r="P61" t="n">
         <v>301</v>
       </c>
+      <c r="Q61" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" t="n">
-        <v>1264</v>
+      <c r="A62" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B62" t="n">
         <v>9955</v>
@@ -4014,10 +4511,18 @@
       <c r="P62" t="n">
         <v>298</v>
       </c>
+      <c r="Q62" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" t="n">
-        <v>1264</v>
+      <c r="A63" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B63" t="n">
         <v>9955</v>
@@ -4072,10 +4577,18 @@
       <c r="P63" t="n">
         <v>297</v>
       </c>
+      <c r="Q63" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="64">
-      <c r="A64" t="n">
-        <v>1264</v>
+      <c r="A64" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B64" t="n">
         <v>9955</v>
@@ -4130,10 +4643,18 @@
       <c r="P64" t="n">
         <v>296</v>
       </c>
+      <c r="Q64" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R64" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="65">
-      <c r="A65" t="n">
-        <v>1264</v>
+      <c r="A65" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B65" t="n">
         <v>9955</v>
@@ -4186,10 +4707,18 @@
       <c r="P65" t="n">
         <v>299</v>
       </c>
+      <c r="Q65" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="66">
-      <c r="A66" t="n">
-        <v>1264</v>
+      <c r="A66" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B66" t="n">
         <v>9955</v>
@@ -4244,10 +4773,18 @@
       <c r="P66" t="n">
         <v>298</v>
       </c>
+      <c r="Q66" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R66" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="67">
-      <c r="A67" t="n">
-        <v>1264</v>
+      <c r="A67" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B67" t="n">
         <v>9955</v>
@@ -4300,10 +4837,18 @@
       <c r="P67" t="n">
         <v>296</v>
       </c>
+      <c r="Q67" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R67" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="68">
-      <c r="A68" t="n">
-        <v>1264</v>
+      <c r="A68" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B68" t="n">
         <v>9955</v>
@@ -4358,10 +4903,18 @@
       <c r="P68" t="n">
         <v>298</v>
       </c>
+      <c r="Q68" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R68" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="69">
-      <c r="A69" t="n">
-        <v>1264</v>
+      <c r="A69" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B69" t="n">
         <v>9955</v>
@@ -4416,10 +4969,18 @@
       <c r="P69" t="n">
         <v>300</v>
       </c>
+      <c r="Q69" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R69" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="70">
-      <c r="A70" t="n">
-        <v>1264</v>
+      <c r="A70" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B70" t="n">
         <v>9955</v>
@@ -4474,10 +5035,18 @@
       <c r="P70" t="n">
         <v>304</v>
       </c>
+      <c r="Q70" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R70" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
+      </c>
     </row>
     <row r="71">
-      <c r="A71" t="n">
-        <v>1264</v>
+      <c r="A71" s="2" t="n">
+        <v>25569.00000000001</v>
       </c>
       <c r="B71" t="n">
         <v>9955</v>
@@ -4531,6 +5100,14 @@
       </c>
       <c r="P71" t="n">
         <v>303</v>
+      </c>
+      <c r="Q71" s="3" t="n">
+        <v>25569</v>
+      </c>
+      <c r="R71" t="inlineStr">
+        <is>
+          <t>00:00:00.000001</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>